<commit_message>
added work of last weeks
</commit_message>
<xml_diff>
--- a/vakken_edited.xlsx
+++ b/vakken_edited.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="25480" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="vakken_edited" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>Vakken voor periode 4</t>
   </si>
@@ -174,18 +174,33 @@
   </si>
   <si>
     <t>Maximale score = 1400 (20 vakken met 2-4 activiteiten die optimaal verdeeld kunnen worden)</t>
+  </si>
+  <si>
+    <t>totaal = 2919</t>
+  </si>
+  <si>
+    <t>Slechts mogelijke score: Subjecten niet verspreid: 43*-10 = 430, 3370 studenten - 20 plaatsen in kleinste lokaaal = 3350, studentenConflict: per vak opgeteld al 1960</t>
+  </si>
+  <si>
+    <t>studenten met minimaal 2 vakken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -209,9 +224,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D37" sqref="A36:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,23 +535,23 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -555,26 +571,38 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <f>IF(B2+C2+E2=2,1,0)</f>
+        <f>B2+C2+E2</f>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>G2-1</f>
         <v>1</v>
       </c>
       <c r="I2">
+        <f>H2*K2</f>
         <v>20</v>
       </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-      <c r="N2">
+      <c r="J2">
+        <f>K2*G2</f>
+        <v>40</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
         <v>10</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>184756</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -594,32 +622,44 @@
         <v>25</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G30" si="0">IF(OR(B3+C3+E3=1,B3+C3+E3=5),1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="G3:G30" si="0">B3+C3+E3</f>
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H30" si="1">G3-1</f>
+        <v>2</v>
       </c>
       <c r="I3">
+        <f t="shared" ref="I3:I30" si="2">H3*K3</f>
+        <v>86</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J30" si="3">K3*G3</f>
+        <v>129</v>
+      </c>
+      <c r="K3">
         <v>43</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>21.5</v>
       </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-      <c r="N3">
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
         <v>21.5</v>
       </c>
-      <c r="P3" s="1">
+      <c r="R3" s="1">
         <v>23100000000000</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="S3" s="1">
         <v>23100000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -642,17 +682,29 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -673,19 +725,31 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I5">
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="K5">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -706,31 +770,43 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I6">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="K6">
         <v>22</v>
       </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-      <c r="K6">
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
         <v>7.33</v>
       </c>
-      <c r="M6">
-        <v>3</v>
-      </c>
-      <c r="N6">
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
         <v>7.33</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>8779605120</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>8779605120</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -751,31 +827,43 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="K7">
         <v>45</v>
       </c>
-      <c r="J7">
-        <v>3</v>
-      </c>
-      <c r="K7">
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
         <v>15</v>
       </c>
-      <c r="M7">
-        <v>3</v>
-      </c>
-      <c r="N7">
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
         <v>15</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <v>5.35E+19</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="S7" s="1">
         <v>5.35E+19</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -796,25 +884,37 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>212</v>
       </c>
       <c r="K8">
+        <v>106</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
         <v>35.33</v>
       </c>
-      <c r="M8" t="s">
-        <v>12</v>
-      </c>
-      <c r="P8" s="1">
+      <c r="O8" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="1">
         <v>1.04E+50</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -835,31 +935,43 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I9">
+        <f t="shared" si="2"/>
+        <v>244</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>305</v>
+      </c>
+      <c r="K9">
         <v>61</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>4</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>15.25</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>4</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>15.25</v>
       </c>
-      <c r="P9" s="1">
+      <c r="R9" s="1">
         <v>1.7399999999999999E+35</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="S9" s="1">
         <v>1.7399999999999999E+35</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -880,31 +992,43 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I10">
+        <f t="shared" si="2"/>
+        <v>207</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>276</v>
+      </c>
+      <c r="K10">
         <v>69</v>
       </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10">
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
         <v>34.5</v>
       </c>
-      <c r="M10">
-        <v>2</v>
-      </c>
-      <c r="N10">
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
         <v>34.5</v>
       </c>
-      <c r="P10" s="1">
+      <c r="R10" s="1">
         <v>1.96E+21</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="S10" s="1">
         <v>1.96E+21</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -927,23 +1051,35 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="J11" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11">
-        <v>3</v>
-      </c>
-      <c r="N11">
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
         <v>13.33</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="S11" s="1">
         <v>3.38E+18</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -964,31 +1100,43 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I12">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="K12">
         <v>27</v>
       </c>
-      <c r="J12">
-        <v>3</v>
-      </c>
-      <c r="K12">
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
         <v>9</v>
       </c>
-      <c r="M12">
-        <v>3</v>
-      </c>
-      <c r="N12">
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
         <v>9</v>
       </c>
-      <c r="P12" s="1">
+      <c r="R12" s="1">
         <v>228000000000</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="S12" s="1">
         <v>228000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1009,25 +1157,37 @@
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I13">
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>144</v>
       </c>
       <c r="K13">
+        <v>72</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
         <v>36</v>
       </c>
-      <c r="M13" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13" s="1">
+      <c r="O13" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" s="1">
         <v>4.43E+20</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1048,25 +1208,37 @@
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I14">
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>88</v>
       </c>
       <c r="K14">
+        <v>44</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
         <v>22</v>
       </c>
-      <c r="M14" t="s">
-        <v>12</v>
-      </c>
-      <c r="P14" s="1">
+      <c r="O14" t="s">
+        <v>12</v>
+      </c>
+      <c r="R14" s="1">
         <v>2100000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1087,25 +1259,37 @@
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I15">
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>64</v>
       </c>
       <c r="K15">
+        <v>32</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
         <v>16</v>
       </c>
-      <c r="M15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P15">
+      <c r="O15" t="s">
+        <v>12</v>
+      </c>
+      <c r="R15">
         <v>601080390</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1126,31 +1310,43 @@
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I16">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="K16">
         <v>21</v>
       </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16">
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
         <v>10.5</v>
       </c>
-      <c r="M16">
-        <v>2</v>
-      </c>
-      <c r="N16">
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
         <v>10.5</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>3879876</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>3879876</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1171,19 +1367,31 @@
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I17">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="K17">
+        <v>25</v>
+      </c>
+      <c r="L17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1204,19 +1412,31 @@
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I18">
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="J18" t="s">
-        <v>12</v>
-      </c>
-      <c r="M18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="K18">
+        <v>84</v>
+      </c>
+      <c r="L18" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1237,19 +1457,31 @@
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I19">
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="J19" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="K19">
+        <v>54</v>
+      </c>
+      <c r="L19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1270,19 +1502,31 @@
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I20">
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="J20" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="K20">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1303,31 +1547,43 @@
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I21">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>162</v>
+      </c>
+      <c r="K21">
         <v>54</v>
       </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-      <c r="K21">
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21">
         <v>18</v>
       </c>
-      <c r="M21">
-        <v>3</v>
-      </c>
-      <c r="N21">
+      <c r="O21">
+        <v>3</v>
+      </c>
+      <c r="P21">
         <v>18</v>
       </c>
-      <c r="P21" s="1">
+      <c r="R21" s="1">
         <v>8.8000000000000003E+23</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="S21" s="1">
         <v>8.8000000000000003E+23</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1350,23 +1606,35 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="J22" t="s">
-        <v>12</v>
-      </c>
-      <c r="M22">
+      <c r="K22">
+        <v>64</v>
+      </c>
+      <c r="L22" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22">
         <v>4</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>16</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="S22" s="1">
         <v>6.6199999999999999E+35</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1389,23 +1657,35 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="J23" t="s">
-        <v>12</v>
-      </c>
-      <c r="M23">
+      <c r="K23">
+        <v>110</v>
+      </c>
+      <c r="L23" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23">
         <v>6</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>18.329999999999998</v>
       </c>
-      <c r="R23" s="1">
+      <c r="T23" s="1">
         <v>2.3099999999999999E+83</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1428,23 +1708,35 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="J24" t="s">
-        <v>12</v>
-      </c>
-      <c r="M24">
-        <v>3</v>
-      </c>
-      <c r="N24">
-        <v>12</v>
-      </c>
-      <c r="Q24" s="1">
+      <c r="K24">
+        <v>36</v>
+      </c>
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24">
+        <v>3</v>
+      </c>
+      <c r="P24">
+        <v>12</v>
+      </c>
+      <c r="S24" s="1">
         <v>3380000000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1467,23 +1759,35 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="J25" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25">
-        <v>3</v>
-      </c>
-      <c r="N25">
+      <c r="K25">
+        <v>44</v>
+      </c>
+      <c r="L25" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25">
+        <v>3</v>
+      </c>
+      <c r="P25">
         <v>14.67</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="S25" s="1">
         <v>4.01E+21</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1504,25 +1808,37 @@
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I26">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>153</v>
+      </c>
+      <c r="K26">
         <v>51</v>
       </c>
-      <c r="J26">
-        <v>3</v>
-      </c>
-      <c r="K26">
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26">
         <v>17</v>
       </c>
-      <c r="M26" t="s">
-        <v>12</v>
-      </c>
-      <c r="P26" s="1">
+      <c r="O26" t="s">
+        <v>12</v>
+      </c>
+      <c r="R26" s="1">
         <v>3.4499999999999999E+22</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1543,31 +1859,43 @@
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I27">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="K27">
         <v>75</v>
       </c>
-      <c r="J27">
-        <v>2</v>
-      </c>
-      <c r="K27">
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
         <v>37.5</v>
       </c>
-      <c r="M27">
-        <v>2</v>
-      </c>
-      <c r="N27">
+      <c r="O27">
+        <v>2</v>
+      </c>
+      <c r="P27">
         <v>37.5</v>
       </c>
-      <c r="P27" s="1">
+      <c r="R27" s="1">
         <v>1.31E+23</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="S27" s="1">
         <v>1.31E+23</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1588,25 +1916,37 @@
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I28">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="K28">
         <v>38</v>
       </c>
-      <c r="J28">
-        <v>2</v>
-      </c>
-      <c r="K28">
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
         <v>19</v>
       </c>
-      <c r="M28" t="s">
-        <v>12</v>
-      </c>
-      <c r="P28">
+      <c r="O28" t="s">
+        <v>12</v>
+      </c>
+      <c r="R28">
         <v>35345263800</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1627,31 +1967,43 @@
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I29">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>156</v>
+      </c>
+      <c r="K29">
         <v>39</v>
       </c>
-      <c r="J29">
-        <v>2</v>
-      </c>
-      <c r="K29">
+      <c r="L29">
+        <v>2</v>
+      </c>
+      <c r="M29">
         <v>19.5</v>
       </c>
-      <c r="M29">
-        <v>2</v>
-      </c>
-      <c r="N29">
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29">
         <v>19.5</v>
       </c>
-      <c r="P29" s="1">
+      <c r="R29" s="1">
         <v>1380000000000</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="S29" s="1">
         <v>1380000000000</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1674,52 +2026,82 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="J30" t="s">
-        <v>12</v>
-      </c>
-      <c r="M30">
-        <v>3</v>
-      </c>
-      <c r="N30">
+      <c r="K30">
+        <v>42</v>
+      </c>
+      <c r="L30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30">
+        <v>3</v>
+      </c>
+      <c r="P30">
         <v>14</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="S30" s="1">
         <v>2.12E+18</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G31">
         <f>SUM(G2:G30)</f>
-        <v>10</v>
-      </c>
-      <c r="P31" s="1">
+        <v>72</v>
+      </c>
+      <c r="H31">
+        <f>SUM(H2:H30)</f>
+        <v>43</v>
+      </c>
+      <c r="I31">
+        <f>SUM(I2:I30)</f>
+        <v>1960</v>
+      </c>
+      <c r="J31">
+        <f>SUM(J2:J30)</f>
+        <v>3370</v>
+      </c>
+      <c r="R31" s="1">
         <v>3.6800000000000002E+301</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="S31" s="1">
         <v>6.1900000000000005E+291</v>
       </c>
-      <c r="R31" s="1">
+      <c r="T31" s="1">
         <v>2.3099999999999999E+83</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>39</v>
       </c>
+      <c r="I32" t="s">
+        <v>51</v>
+      </c>
       <c r="J32">
+        <v>406</v>
+      </c>
+      <c r="L32">
         <v>40</v>
       </c>
-      <c r="M32">
+      <c r="O32">
         <v>50</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1729,8 +2111,14 @@
       <c r="D33" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1743,29 +2131,68 @@
       <c r="F34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P35">
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <v>38</v>
+      </c>
+      <c r="R35">
         <v>52.762</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P36">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36">
+        <f>SUM(J31:J35)</f>
+        <v>4171</v>
+      </c>
+      <c r="R36">
         <v>676</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37">
+        <f>H31*-10-I31-(J36-20)</f>
+        <v>-6541</v>
+      </c>
+      <c r="C37">
+        <v>1440</v>
+      </c>
+      <c r="D37">
+        <f>-B37+C37</f>
+        <v>7981</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>